<commit_message>
updated test results for short
</commit_message>
<xml_diff>
--- a/Tests/baseline_short_sma_5_25_AA.xlsx
+++ b/Tests/baseline_short_sma_5_25_AA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Windows\Documents\bt_plat\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D71AE1-28A8-4E40-884E-37580CCD241E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B8EF19-535B-4A54-82F3-24791CF4817D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="22">
   <si>
     <t>Symbol</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>Open Short</t>
+  </si>
+  <si>
+    <t>Open</t>
   </si>
 </sst>
 </file>
@@ -2710,8 +2713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F3CDDA-1C26-400D-9B56-CE43A1C5EFCC}">
   <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4403,7 +4406,7 @@
         <v>17</v>
       </c>
       <c r="B43" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C43" s="1">
         <v>43301</v>
@@ -4411,8 +4414,8 @@
       <c r="D43">
         <v>40.31</v>
       </c>
-      <c r="E43" s="1">
-        <v>43325</v>
+      <c r="E43" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="F43">
         <v>44.46</v>

</xml_diff>